<commit_message>
Added Apach POI reading excel workbook demo source code.
</commit_message>
<xml_diff>
--- a/SeleniumTraining/config.xlsx
+++ b/SeleniumTraining/config.xlsx
@@ -1,37 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanrustrainingcentre/Development/selenium-training-may212018/SeleniumTraining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A13CCC3-A2AB-8C47-98D4-A56C97B4EA90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0EBD66-DC77-8B42-809F-5852B819C33C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="-11540" windowWidth="28040" windowHeight="11540" activeTab="1" xr2:uid="{3C73E29C-37C5-C648-B2C4-0F610F56A0CA}"/>
+    <workbookView xWindow="3800" yWindow="-13220" windowWidth="20480" windowHeight="11540" xr2:uid="{3C73E29C-37C5-C648-B2C4-0F610F56A0CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="ENV" sheetId="1" r:id="rId1"/>
+    <sheet name="ENV_URLS" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage_Elements" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>QA1_URL</t>
   </si>
@@ -67,13 +64,36 @@
   </si>
   <si>
     <t>&lt;div id="header_text_id"&gt;Header Text&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>asdfasdfas</t>
+  </si>
+  <si>
+    <t>asdfadfas</t>
+  </si>
+  <si>
+    <t>asdfasdfa</t>
+  </si>
+  <si>
+    <t>asdfasdfas 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,13 +119,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,14 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9DE5AF-32E9-3E48-81A5-B56974B4DAA4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -442,6 +466,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>SUM(A8:A9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -451,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A906605-88CB-4740-B6E5-31355E19DB85}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,4 +574,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DE3DDC-4B47-6C41-A4AE-ED783EAE5993}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DFD3E2-33ED-9E41-A667-EF03CE274F9B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>